<commit_message>
Eighteen test cases completed
</commit_message>
<xml_diff>
--- a/testData/invalidUserCredentials.xlsx
+++ b/testData/invalidUserCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2464049\IdeaProjects\Decathlon_final_project_team2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664DFD95-8624-4BE8-9D54-09346FB5C591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2C5E05-CDCA-4CC4-AA81-42BD2E6EB479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A87BFB4A-E5EB-4064-A578-5DA69F9A38D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Email</t>
   </si>
@@ -53,7 +53,10 @@
     <t>demo3@gmail.com</t>
   </si>
   <si>
-    <t>demo4@gmail.com</t>
+    <t>demo4@yahoo.com</t>
+  </si>
+  <si>
+    <t>demo5@cts.com</t>
   </si>
 </sst>
 </file>
@@ -474,11 +477,13 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>